<commit_message>
Added landing performance file
</commit_message>
<xml_diff>
--- a/data/performance_data.xlsx
+++ b/data/performance_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Desktop\Projects\Performance Cessna 172N\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA64859B-2C81-42F5-B03D-4D815B837565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1954A6-7C48-4D4A-9E03-00D26AD89A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="3" xr2:uid="{C5F2153C-1967-4E78-80FB-B64280FCE72E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{C5F2153C-1967-4E78-80FB-B64280FCE72E}"/>
   </bookViews>
   <sheets>
     <sheet name="takeoff" sheetId="2" r:id="rId1"/>
@@ -3388,7 +3388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0EA5-94ED-4AB1-8E11-44973D071098}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -5239,8 +5239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18DDF38-2D48-42EF-A6EB-F074020E8AB7}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5254,10 +5254,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -5291,11 +5291,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -5329,11 +5329,11 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1000</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>218</v>
@@ -5367,11 +5367,11 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2000</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>220</v>
@@ -5405,11 +5405,11 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3000</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>224</v>
@@ -5443,11 +5443,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4000</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>193</v>
@@ -5481,11 +5481,11 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5000</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -5519,11 +5519,11 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="1">
+        <v>6000</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B8" s="1">
-        <v>6000</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>233</v>
@@ -5557,11 +5557,11 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="1">
+        <v>7000</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7000</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>242</v>
@@ -5595,11 +5595,11 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B10" s="1">
-        <v>8000</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
Updated takeoff.py docstring and cruise.py code and docstring
</commit_message>
<xml_diff>
--- a/data/performance_data.xlsx
+++ b/data/performance_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Desktop\Projects\Performance Cessna 172N\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1954A6-7C48-4D4A-9E03-00D26AD89A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583F6342-6C91-4B59-9B72-756E1BF81AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{C5F2153C-1967-4E78-80FB-B64280FCE72E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{C5F2153C-1967-4E78-80FB-B64280FCE72E}"/>
   </bookViews>
   <sheets>
     <sheet name="takeoff" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="358">
   <si>
     <t>weight</t>
   </si>
@@ -551,18 +551,6 @@
     <t>43</t>
   </si>
   <si>
-    <t>75_bhp</t>
-  </si>
-  <si>
-    <t>65_bhp</t>
-  </si>
-  <si>
-    <t>55_bhp</t>
-  </si>
-  <si>
-    <t>45_bhp</t>
-  </si>
-  <si>
     <t>471</t>
   </si>
   <si>
@@ -1128,6 +1116,9 @@
   </si>
   <si>
     <t>7.85</t>
+  </si>
+  <si>
+    <t>65</t>
   </si>
 </sst>
 </file>
@@ -2785,7 +2776,7 @@
         <v>3000</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2793,7 +2784,7 @@
         <v>4000</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2801,7 +2792,7 @@
         <v>5000</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2809,7 +2800,7 @@
         <v>6000</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2817,7 +2808,7 @@
         <v>7000</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2825,7 +2816,7 @@
         <v>8000</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2833,7 +2824,7 @@
         <v>9000</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2841,7 +2832,7 @@
         <v>10000</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2849,7 +2840,7 @@
         <v>11000</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2857,7 +2848,7 @@
         <v>12000</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2870,7 +2861,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3097,7 +3088,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
@@ -3120,7 +3111,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>66</v>
@@ -3143,7 +3134,7 @@
         <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>69</v>
@@ -3166,7 +3157,7 @@
         <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>74</v>
@@ -3189,7 +3180,7 @@
         <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>78</v>
@@ -3212,7 +3203,7 @@
         <v>78</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>81</v>
@@ -3235,7 +3226,7 @@
         <v>81</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>82</v>
@@ -3258,7 +3249,7 @@
         <v>82</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>60</v>
@@ -3281,7 +3272,7 @@
         <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>85</v>
@@ -3304,7 +3295,7 @@
         <v>89</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>90</v>
@@ -3327,7 +3318,7 @@
         <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>94</v>
@@ -3350,7 +3341,7 @@
         <v>98</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>99</v>
@@ -3373,7 +3364,7 @@
         <v>102</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>103</v>
@@ -3455,7 +3446,7 @@
         <v>115</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>32</v>
@@ -3464,7 +3455,7 @@
         <v>116</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3481,7 +3472,7 @@
         <v>111</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>52</v>
@@ -3490,7 +3481,7 @@
         <v>117</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>118</v>
@@ -3499,7 +3490,7 @@
         <v>119</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3516,7 +3507,7 @@
         <v>106</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>120</v>
@@ -3525,7 +3516,7 @@
         <v>121</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>122</v>
@@ -3534,7 +3525,7 @@
         <v>121</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3551,7 +3542,7 @@
         <v>101</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>123</v>
@@ -3560,7 +3551,7 @@
         <v>124</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>125</v>
@@ -3569,7 +3560,7 @@
         <v>126</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3586,7 +3577,7 @@
         <v>95</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>127</v>
@@ -3595,7 +3586,7 @@
         <v>128</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>129</v>
@@ -3604,7 +3595,7 @@
         <v>130</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3630,7 +3621,7 @@
         <v>131</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>32</v>
@@ -3639,7 +3630,7 @@
         <v>131</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3656,7 +3647,7 @@
         <v>116</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>32</v>
@@ -3665,7 +3656,7 @@
         <v>116</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>52</v>
@@ -3674,7 +3665,7 @@
         <v>116</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3691,7 +3682,7 @@
         <v>111</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>132</v>
@@ -3700,7 +3691,7 @@
         <v>119</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>120</v>
@@ -3709,7 +3700,7 @@
         <v>133</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3726,7 +3717,7 @@
         <v>105</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>134</v>
@@ -3735,7 +3726,7 @@
         <v>121</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>135</v>
@@ -3744,7 +3735,7 @@
         <v>136</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3761,7 +3752,7 @@
         <v>100</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>137</v>
@@ -3770,7 +3761,7 @@
         <v>126</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>138</v>
@@ -3779,7 +3770,7 @@
         <v>139</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3796,7 +3787,7 @@
         <v>94</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>140</v>
@@ -3805,7 +3796,7 @@
         <v>130</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>141</v>
@@ -3814,7 +3805,7 @@
         <v>142</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3840,7 +3831,7 @@
         <v>143</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>32</v>
@@ -3849,7 +3840,7 @@
         <v>143</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3866,7 +3857,7 @@
         <v>116</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>52</v>
@@ -3875,7 +3866,7 @@
         <v>116</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>132</v>
@@ -3884,7 +3875,7 @@
         <v>144</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3901,7 +3892,7 @@
         <v>110</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>120</v>
@@ -3910,7 +3901,7 @@
         <v>133</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>134</v>
@@ -3919,7 +3910,7 @@
         <v>133</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3936,7 +3927,7 @@
         <v>105</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>135</v>
@@ -3945,7 +3936,7 @@
         <v>136</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>145</v>
@@ -3954,7 +3945,7 @@
         <v>146</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -3971,7 +3962,7 @@
         <v>99</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>147</v>
@@ -3980,7 +3971,7 @@
         <v>139</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>127</v>
@@ -3989,7 +3980,7 @@
         <v>148</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4006,7 +3997,7 @@
         <v>93</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>141</v>
@@ -4015,7 +4006,7 @@
         <v>142</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>149</v>
@@ -4024,7 +4015,7 @@
         <v>150</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -4050,7 +4041,7 @@
         <v>151</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>32</v>
@@ -4059,7 +4050,7 @@
         <v>151</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -4076,7 +4067,7 @@
         <v>120</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>32</v>
@@ -4085,7 +4076,7 @@
         <v>143</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>52</v>
@@ -4094,7 +4085,7 @@
         <v>152</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -4111,7 +4102,7 @@
         <v>115</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>132</v>
@@ -4120,7 +4111,7 @@
         <v>144</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>120</v>
@@ -4129,7 +4120,7 @@
         <v>153</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -4146,7 +4137,7 @@
         <v>110</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>154</v>
@@ -4155,7 +4146,7 @@
         <v>133</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>155</v>
@@ -4164,7 +4155,7 @@
         <v>156</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -4181,7 +4172,7 @@
         <v>104</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>145</v>
@@ -4190,7 +4181,7 @@
         <v>146</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>125</v>
@@ -4199,7 +4190,7 @@
         <v>157</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -4216,7 +4207,7 @@
         <v>98</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>127</v>
@@ -4225,7 +4216,7 @@
         <v>148</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>129</v>
@@ -4234,7 +4225,7 @@
         <v>158</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -4251,7 +4242,7 @@
         <v>122</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>32</v>
@@ -4260,7 +4251,7 @@
         <v>151</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>52</v>
@@ -4269,7 +4260,7 @@
         <v>159</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -4286,7 +4277,7 @@
         <v>120</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>48</v>
@@ -4295,7 +4286,7 @@
         <v>152</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>132</v>
@@ -4304,7 +4295,7 @@
         <v>131</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -4321,7 +4312,7 @@
         <v>114</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>160</v>
@@ -4330,7 +4321,7 @@
         <v>144</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>154</v>
@@ -4339,7 +4330,7 @@
         <v>161</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -4356,7 +4347,7 @@
         <v>109</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>155</v>
@@ -4365,7 +4356,7 @@
         <v>156</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>145</v>
@@ -4374,7 +4365,7 @@
         <v>162</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -4391,7 +4382,7 @@
         <v>103</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>125</v>
@@ -4400,7 +4391,7 @@
         <v>157</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>138</v>
@@ -4409,7 +4400,7 @@
         <v>163</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4426,7 +4417,7 @@
         <v>97</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>129</v>
@@ -4435,7 +4426,7 @@
         <v>158</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>141</v>
@@ -4444,7 +4435,7 @@
         <v>164</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -4461,7 +4452,7 @@
         <v>119</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>132</v>
@@ -4470,7 +4461,7 @@
         <v>131</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>160</v>
@@ -4479,7 +4470,7 @@
         <v>165</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -4496,7 +4487,7 @@
         <v>114</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>154</v>
@@ -4505,7 +4496,7 @@
         <v>153</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>155</v>
@@ -4514,7 +4505,7 @@
         <v>117</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -4531,7 +4522,7 @@
         <v>108</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>123</v>
@@ -4540,7 +4531,7 @@
         <v>162</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>137</v>
@@ -4549,7 +4540,7 @@
         <v>166</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -4566,7 +4557,7 @@
         <v>102</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>138</v>
@@ -4575,7 +4566,7 @@
         <v>163</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>140</v>
@@ -4584,7 +4575,7 @@
         <v>124</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -4601,7 +4592,7 @@
         <v>96</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>141</v>
@@ -4610,7 +4601,7 @@
         <v>164</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>167</v>
@@ -4619,7 +4610,7 @@
         <v>128</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4631,11 +4622,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD163B00-9F32-4E0A-9B28-C44F9ADCF431}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4643,16 +4634,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>357</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4660,13 +4651,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>76</v>
@@ -4677,13 +4668,13 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>76</v>
@@ -4694,13 +4685,13 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>76</v>
@@ -4711,13 +4702,13 @@
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>76</v>
@@ -4728,16 +4719,16 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4745,16 +4736,16 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4762,16 +4753,16 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4785,9 +4776,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.5546875" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4795,16 +4786,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>357</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4812,16 +4803,16 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4829,16 +4820,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4846,16 +4837,16 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -4863,16 +4854,16 @@
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4880,16 +4871,16 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4897,16 +4888,16 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4914,16 +4905,16 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4937,9 +4928,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.88671875" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4947,16 +4938,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>357</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4964,16 +4955,16 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4981,16 +4972,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4998,16 +4989,16 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -5015,16 +5006,16 @@
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -5032,16 +5023,16 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -5049,16 +5040,16 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -5066,16 +5057,16 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5089,9 +5080,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.6640625" style="2"/>
+    <col min="1" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -5099,16 +5090,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>357</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -5116,16 +5107,16 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -5133,16 +5124,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -5150,16 +5141,16 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -5167,16 +5158,16 @@
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -5184,16 +5175,16 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -5201,16 +5192,16 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -5218,16 +5209,16 @@
         <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -5239,8 +5230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18DDF38-2D48-42EF-A6EB-F074020E8AB7}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5257,7 +5248,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -5301,31 +5292,31 @@
         <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -5336,34 +5327,34 @@
         <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -5374,34 +5365,34 @@
         <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -5412,34 +5403,34 @@
         <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -5450,34 +5441,34 @@
         <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -5491,31 +5482,31 @@
         <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -5526,34 +5517,34 @@
         <v>120</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -5564,34 +5555,34 @@
         <v>120</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -5602,34 +5593,34 @@
         <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the option to select input and output path
</commit_message>
<xml_diff>
--- a/data/performance_data.xlsx
+++ b/data/performance_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Desktop\Projects\Performance Cessna 172N\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583F6342-6C91-4B59-9B72-756E1BF81AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C7CDF4-3E37-467A-B7CB-6AD167C5C122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{C5F2153C-1967-4E78-80FB-B64280FCE72E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{C5F2153C-1967-4E78-80FB-B64280FCE72E}"/>
   </bookViews>
   <sheets>
     <sheet name="takeoff" sheetId="2" r:id="rId1"/>
@@ -4622,7 +4622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD163B00-9F32-4E0A-9B28-C44F9ADCF431}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4926,7 +4926,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D8AEED-E4CD-42A4-8921-96A462329D2D}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>